<commit_message>
Implemented conversion properties->xlsx. Working.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/messages.xlsx
+++ b/src/test/resources/data/messages.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="messages" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">home.greetings</t>
   </si>
   <si>
-    <t xml:space="preserve">Hallo und willkommen zurück!</t>
+    <t xml:space="preserve">Hallo und willkommen!</t>
   </si>
   <si>
     <t xml:space="preserve">Hello and welcome back!</t>
@@ -67,6 +67,15 @@
     <t xml:space="preserve">Administrateur</t>
   </si>
   <si>
+    <t xml:space="preserve">user.client.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client</t>
+  </si>
+  <si>
     <t xml:space="preserve">user.manager.title</t>
   </si>
   <si>
@@ -74,15 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gestionnaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user.client.title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Klient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Client</t>
   </si>
 </sst>
 </file>
@@ -97,6 +97,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -118,6 +119,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,22 +190,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -214,7 +216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
@@ -228,7 +230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -242,7 +244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
@@ -264,7 +266,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>17</v>
@@ -278,12 +280,13 @@
         <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>